<commit_message>
delete trash excel file
</commit_message>
<xml_diff>
--- a/Paper INFO.xlsx
+++ b/Paper INFO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Phan\Desktop\Bach Khoa Studies\HK242\MP - Information Systems\Multidisciplinary-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07A8945-5A0D-4971-816C-EE0092E60BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDEE538-6E64-497D-AAB2-DADD80FEB182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Citation</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>Anomaly data points are not detected since they are calculated into the compressed value; sensitive with skewed data</t>
+  </si>
+  <si>
+    <t>Improved Piecewise Constant Approximation \n Method for Compressing Data Streams</t>
+  </si>
+  <si>
+    <t>Atik Mahbub, Farhana Haque, Habibul Bashar, Mohammad Rezwanul Huq</t>
+  </si>
+  <si>
+    <t>The paper proposed a new compression method based on PCA and APCA. In detail, they use PCA for compressing fixed-size windows that don’t violate the compression condition (Merge Phase), and use APCA to deal with the data points in the window that violates the compression condition (Split Phase)</t>
+  </si>
+  <si>
+    <t>Make use of advantages of PCA and APCA, improve their weaknesses when dealing with skewed data</t>
   </si>
 </sst>
 </file>
@@ -569,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -581,7 +593,7 @@
     <col min="4" max="4" width="8.8984375" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.8984375" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.09765625" style="11" customWidth="1"/>
     <col min="8" max="8" width="34.5" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.8984375" style="9" bestFit="1" customWidth="1"/>
@@ -646,7 +658,7 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="2:13" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="210" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -666,10 +678,10 @@
       <c r="H5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K5" s="5"/>
@@ -697,16 +709,26 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="189" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="8"/>
+      <c r="E7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2019</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -2627,8 +2649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08F07AF-3552-413A-9019-A8AE1AC08F0E}">
   <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Update result for PMC-MR, PMC-Mean
</commit_message>
<xml_diff>
--- a/Paper INFO.xlsx
+++ b/Paper INFO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Phan\Desktop\Bach Khoa Studies\HK242\MP - Information Systems\Multidisciplinary-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDEE538-6E64-497D-AAB2-DADD80FEB182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E0190-4FEE-49D5-B5CA-F400ECB3877F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Citation</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>Make use of advantages of PCA and APCA, improve their weaknesses when dealing with skewed data</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Compressed until the max - min &gt; 2 \epsilon</t>
+  </si>
+  <si>
+    <t>Compressed until the mean of observed points is far from max (or mean)</t>
   </si>
 </sst>
 </file>
@@ -243,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -282,22 +291,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -595,8 +601,8 @@
     <col min="6" max="6" width="6.296875" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.09765625" style="11" customWidth="1"/>
     <col min="8" max="8" width="34.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.8984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.796875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="23.69921875" style="9" customWidth="1"/>
     <col min="11" max="16384" width="8.796875" style="9"/>
   </cols>
   <sheetData>
@@ -709,7 +715,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="2:13" ht="189" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="126" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -2647,44 +2653,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08F07AF-3552-413A-9019-A8AE1AC08F0E}">
-  <dimension ref="B2:D7"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="8.796875" style="12"/>
-    <col min="2" max="2" width="12.796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.8984375" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="12" customWidth="1"/>
+    <col min="2" max="2" width="14.796875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="42.19921875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="41.19921875" style="12" customWidth="1"/>
     <col min="5" max="16384" width="8.796875" style="12"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:4" ht="38.4" x14ac:dyDescent="0.5">
+      <c r="B3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B4" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B4" s="15" t="s">
-        <v>20</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>22</v>
@@ -2693,32 +2699,43 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="57.6" x14ac:dyDescent="0.5">
-      <c r="B5" s="16" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.5">
+      <c r="B6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D6" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B6" s="17"/>
-      <c r="C6" s="13" t="s">
+    <row r="7" spans="2:4" ht="38.4" x14ac:dyDescent="0.5">
+      <c r="B7" s="16"/>
+      <c r="C7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B7" s="18"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B8" s="17"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Summarize for Chebyshev Compression
</commit_message>
<xml_diff>
--- a/Paper INFO.xlsx
+++ b/Paper INFO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Phan\Desktop\Bach Khoa Studies\HK242\MP - Information Systems\Multidisciplinary-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E0190-4FEE-49D5-B5CA-F400ECB3877F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED46F6FA-6CCB-448F-90D6-937F1DA38F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Citation</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Compressed until the mean of observed points is far from max (or mean)</t>
+  </si>
+  <si>
+    <t>The paper aims to find out the optimal block size for leveraging the power of Chebyshev Compression, as well as the ideal value for threshold</t>
+  </si>
+  <si>
+    <t>The concepts of Chebyshev compression, optimal block size strategy using recursion, with the insight that data points that have related information according to their difference should be compressed together, and increase the block size to compress all of them, and vice versa.</t>
   </si>
 </sst>
 </file>
@@ -587,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="76" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -664,7 +670,7 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="2:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="126" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -694,7 +700,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="2:13" ht="84" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="210" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -708,7 +714,12 @@
       <c r="F6" s="5">
         <v>2015</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>

</xml_diff>

<commit_message>
Presentation for Midterm Seminar
</commit_message>
<xml_diff>
--- a/Paper INFO.xlsx
+++ b/Paper INFO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Phan\Desktop\Bach Khoa Studies\HK242\MP - Information Systems\Multidisciplinary-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED46F6FA-6CCB-448F-90D6-937F1DA38F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563759FA-039A-495E-B9A7-CD8E22FAE58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28898" yWindow="-5955" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -97,18 +97,9 @@
     <t>O(1)</t>
   </si>
   <si>
-    <t>Những điểm dữ liệu bất thường qua từng giai đoạn không được phát hiện do bị chuyển thành giá trị chung</t>
-  </si>
-  <si>
-    <t>Các điểm dữ liệu có sự chênh lệch quá lớn -&gt; Error sát với threshold</t>
-  </si>
-  <si>
     <t>PMC-Mean</t>
   </si>
   <si>
-    <t>Sinh ra nhiều segment hơn so với PMC-MR</t>
-  </si>
-  <si>
     <t>Learn PMC and its variant (PMC-MR, PMC-Mean), Identifying Cons of PMC-MR and PMC-Mean</t>
   </si>
   <si>
@@ -127,22 +118,32 @@
     <t>The paper proposed a new compression method based on PCA and APCA. In detail, they use PCA for compressing fixed-size windows that don’t violate the compression condition (Merge Phase), and use APCA to deal with the data points in the window that violates the compression condition (Split Phase)</t>
   </si>
   <si>
-    <t>Make use of advantages of PCA and APCA, improve their weaknesses when dealing with skewed data</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Compressed until the max - min &gt; 2 \epsilon</t>
   </si>
   <si>
-    <t>Compressed until the mean of observed points is far from max (or mean)</t>
-  </si>
-  <si>
     <t>The paper aims to find out the optimal block size for leveraging the power of Chebyshev Compression, as well as the ideal value for threshold</t>
   </si>
   <si>
     <t>The concepts of Chebyshev compression, optimal block size strategy using recursion, with the insight that data points that have related information according to their difference should be compressed together, and increase the block size to compress all of them, and vice versa.</t>
+  </si>
+  <si>
+    <t>Make use of advantages of PCA and APCA, improve their weaknesses when dealing with skewed data (Hybrid PCA)</t>
+  </si>
+  <si>
+    <t>Anomalous data points at each stage are not detected as they are converted into common values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data points with excessively large deviations → Error close to the threshold.
+</t>
+  </si>
+  <si>
+    <t>Create more segments</t>
+  </si>
+  <si>
+    <t>Compressed until the mean of observed points is far from max (or min)</t>
   </si>
 </sst>
 </file>
@@ -194,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -245,10 +246,23 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -258,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,13 +316,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -593,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="76" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScale="76" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -688,13 +705,13 @@
         <v>13</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -715,10 +732,10 @@
         <v>2015</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -731,20 +748,20 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F7" s="5">
         <v>2019</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -2664,10 +2681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08F07AF-3552-413A-9019-A8AE1AC08F0E}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.5"/>
@@ -2685,18 +2702,18 @@
         <v>21</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="38.4" x14ac:dyDescent="0.5">
       <c r="B3" s="14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.5">
@@ -2721,32 +2738,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="57.6" x14ac:dyDescent="0.5">
-      <c r="B6" s="15" t="s">
+    <row r="6" spans="2:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>23</v>
+      <c r="C6" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="38.4" x14ac:dyDescent="0.5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B8" s="17"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="18"/>
+      <c r="C7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>